<commit_message>
Add the cannon sheet Add the confirmation for the modification. Add the time/money spend in modification
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="25120" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="8480" yWindow="400" windowWidth="25120" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="defaultDialog.csv" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,8 @@
           <t>没有人讲话
 1：普通npc
 2：城市npc
-3: 某职业的npc</t>
+3: 某职业的npc
+4: 船长</t>
         </r>
       </text>
     </comment>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>int</t>
   </si>
@@ -182,6 +183,15 @@
   </si>
   <si>
     <t>dialog_lose_friend</t>
+  </si>
+  <si>
+    <t>name_shipyard_owner</t>
+  </si>
+  <si>
+    <t>dialog_modify_ship_confirm</t>
+  </si>
+  <si>
+    <t>dialog_no_enough_money</t>
   </si>
 </sst>
 </file>
@@ -614,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -808,6 +818,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Almost finish ship modify function And change the ship data structure. And the modification ability will be compute to get it.
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="400" windowWidth="25120" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="8480" yWindow="400" windowWidth="36200" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="defaultDialog.csv" sheetId="1" r:id="rId1"/>
@@ -627,7 +627,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Add limit for sailor, small change on the money
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="400" windowWidth="36200" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="1840" yWindow="3500" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="defaultDialog.csv" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>int</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>dialog_no_enough_money</t>
+  </si>
+  <si>
+    <t>dialog_fill_food</t>
+  </si>
+  <si>
+    <t>name_dock_sailor</t>
+  </si>
+  <si>
+    <t>dialog_no_sailors</t>
   </si>
 </sst>
 </file>
@@ -260,8 +269,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -280,7 +291,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -288,6 +299,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -295,6 +307,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -624,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -858,6 +871,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add food and sailor check, and begin to add hire sailors
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>int</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>dialog_no_sailors</t>
+  </si>
+  <si>
+    <t>dialog_no_enough_sailors</t>
+  </si>
+  <si>
+    <t>dialog_checkout_food</t>
+  </si>
+  <si>
+    <t>dialog_checkout_food_not_enough</t>
   </si>
 </sst>
 </file>
@@ -269,8 +278,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,7 +308,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -300,6 +317,10 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -308,6 +329,10 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -637,15 +662,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -908,6 +933,66 @@
         <v>22</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make dialog in a unit way
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>int</t>
   </si>
@@ -228,13 +228,40 @@
   </si>
   <si>
     <t>dialog_hire_continue_need</t>
+  </si>
+  <si>
+    <t>dialog_invest_success</t>
+  </si>
+  <si>
+    <t>dialog_signup_failure_full</t>
+  </si>
+  <si>
+    <t>dialog_signup_start</t>
+  </si>
+  <si>
+    <t>name_governor</t>
+  </si>
+  <si>
+    <t>dialog_need_to_sign_before_exchange</t>
+  </si>
+  <si>
+    <t>dialog_no_ship_to_sale</t>
+  </si>
+  <si>
+    <t>dialog_no_ship_no_game</t>
+  </si>
+  <si>
+    <t>dialog_military_invest_start</t>
+  </si>
+  <si>
+    <t>dialog_more_free_sailors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,6 +305,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -296,7 +331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -338,11 +373,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +415,14 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -383,6 +443,14 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -712,15 +780,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:F22"/>
+      <selection activeCell="B30" sqref="B30:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1163,6 +1231,166 @@
         <v>22</v>
       </c>
       <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Equip Role - part 1
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujiel/Documents/mygit/SailingGame/DataSource/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="3500" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="17880" yWindow="5140" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="defaultDialog.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="defaultDialog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -18,118 +26,29 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Yujie Liu</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-0: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t>没有人讲话
-1：普通npc
-2：城市npc
-3: 某职业的npc
-4: 船长</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-0</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t>：无人说话
-type = 1：npcId
-type = 2：建筑物Id
-type = 3： job id</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-if npcType = 0, then use this
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+  <si>
+    <t>dialogId</t>
+  </si>
+  <si>
+    <t>npcType</t>
+  </si>
+  <si>
+    <t>npcParameter</t>
+  </si>
+  <si>
+    <t>photoId</t>
+  </si>
+  <si>
+    <t>dialogName</t>
+  </si>
+  <si>
+    <t>backgroundId</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>int</t>
   </si>
@@ -137,39 +56,18 @@
     <t>string</t>
   </si>
   <si>
-    <t>dialogId</t>
-  </si>
-  <si>
-    <t>photoId</t>
-  </si>
-  <si>
-    <t>dialogName</t>
-  </si>
-  <si>
-    <t>backgroundId</t>
-  </si>
-  <si>
-    <t>npcType</t>
-  </si>
-  <si>
-    <t>npcParameter</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>dialog_new_item_discover</t>
   </si>
   <si>
+    <t>name_exchange_owner</t>
+  </si>
+  <si>
+    <t>dialog_buy_item</t>
+  </si>
+  <si>
     <t>name_shop_owner</t>
   </si>
   <si>
-    <t>dialog_buy_item</t>
-  </si>
-  <si>
-    <t>name_exchange_owner</t>
-  </si>
-  <si>
     <t>dialog_sell_item</t>
   </si>
   <si>
@@ -185,12 +83,12 @@
     <t>dialog_lose_friend</t>
   </si>
   <si>
+    <t>dialog_modify_ship_confirm</t>
+  </si>
+  <si>
     <t>name_shipyard_owner</t>
   </si>
   <si>
-    <t>dialog_modify_ship_confirm</t>
-  </si>
-  <si>
     <t>dialog_no_enough_money</t>
   </si>
   <si>
@@ -233,15 +131,15 @@
     <t>dialog_invest_success</t>
   </si>
   <si>
+    <t>name_governor</t>
+  </si>
+  <si>
     <t>dialog_signup_failure_full</t>
   </si>
   <si>
     <t>dialog_signup_start</t>
   </si>
   <si>
-    <t>name_governor</t>
-  </si>
-  <si>
     <t>dialog_need_to_sign_before_exchange</t>
   </si>
   <si>
@@ -255,58 +153,29 @@
   </si>
   <si>
     <t>dialog_more_free_sailors</t>
+  </si>
+  <si>
+    <t>dialog_new_ship_into_dock</t>
+  </si>
+  <si>
+    <t>dialog_equip_an_equipment</t>
+  </si>
+  <si>
+    <t>dialog_cannot_equip</t>
+  </si>
+  <si>
+    <t>dialog_i_cannot_equip</t>
+  </si>
+  <si>
+    <t>dialog_unequip_an_equipment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -331,130 +200,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -469,44 +230,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -536,12 +297,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -580,229 +341,168 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:F30"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -814,27 +514,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -848,13 +548,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -868,13 +568,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -888,13 +588,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -914,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -934,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -954,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -974,9 +674,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -988,13 +688,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1034,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1054,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1074,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1094,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1114,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1134,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1174,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1194,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1214,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1234,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1248,15 +948,15 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1268,15 +968,15 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>36</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>35</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1288,13 +988,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1308,13 +1008,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1334,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1354,8 +1054,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>40</v>
       </c>
       <c r="B29">
@@ -1368,13 +1068,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1394,14 +1094,107 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add menu button in the game
</commit_message>
<xml_diff>
--- a/DataSource/excel/defaultDialog.xlsx
+++ b/DataSource/excel/defaultDialog.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujiel/Documents/mygit/SailingGame/DataSource/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="46200" yWindow="8800" windowWidth="28800" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="defaultDialog.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>dialogId</t>
   </si>
@@ -204,18 +199,40 @@
   </si>
   <si>
     <t>dialog_days_not_enough_to_sail</t>
+  </si>
+  <si>
+    <t>dialog_back_to_menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,13 +253,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -298,7 +319,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -333,7 +354,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -510,7 +531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -518,19 +539,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -570,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -590,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -610,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -630,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -650,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -670,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -690,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -710,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -730,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -750,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -770,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -790,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -810,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -830,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -850,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -870,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -890,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -910,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -930,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -950,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -970,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -990,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1010,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1030,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1050,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1070,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1090,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1110,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1130,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1150,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1170,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1210,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1230,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1290,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1310,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1330,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -1350,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1370,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1390,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1430,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1450,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1470,7 +1491,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>